<commit_message>
- files for H and G
</commit_message>
<xml_diff>
--- a/wwlLancMsc_data/dataDictionary.xlsx
+++ b/wwlLancMsc_data/dataDictionary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="8_{AC18906E-F7C5-4E1E-BFF7-B27552C193E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{028005B9-A3B6-476B-8FB8-CA26C193156F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{290F325C-FF08-46D0-8C78-02E0FDA84A53}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{290F325C-FF08-46D0-8C78-02E0FDA84A53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>site_national_code</t>
   </si>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DE5673-06FD-47FA-8861-7B0812E54659}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>